<commit_message>
add pandas,numpy, update str
</commit_message>
<xml_diff>
--- a/dbTask.xlsx
+++ b/dbTask.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4170" yWindow="1590" windowWidth="20880" windowHeight="11835" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Datos del crud" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Datos del crud" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -484,7 +484,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tarea a</t>
+          <t>Taraea actualizada</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>En espera</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,6 @@
     <row r="9">
       <c r="J9" s="1" t="n"/>
     </row>
-    <row r="10"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>